<commit_message>
supp + ini case
</commit_message>
<xml_diff>
--- a/map.xlsx
+++ b/map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loic-\OneDrive\Documents\GitHub\Projet-LO43\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{431F26AD-9D92-4329-AA84-9983D88D7D24}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{350C181F-C796-46E6-8238-308B8E674AD7}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="8_{431F26AD-9D92-4329-AA84-9983D88D7D24}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{586435DC-6378-401E-9429-8A3EA98F0C6B}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" xr2:uid="{CBC8F156-E23D-49EC-AAE8-3A0909B6DE8A}"/>
   </bookViews>
@@ -116,7 +116,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -263,10 +263,30 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
         <color indexed="64"/>
       </right>
+      <top/>
+      <bottom style="dashDotDot">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thick">
         <color indexed="64"/>
       </top>
@@ -274,55 +294,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thick">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thick">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="dashDotDot">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thick">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thick">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color indexed="64"/>
-      </left>
-      <right style="thick">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -332,7 +308,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -362,7 +338,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -386,19 +362,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -424,7 +394,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -743,12 +713,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{324130C1-EECB-42D2-B35E-2270306D22B0}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="2.21875" customWidth="1"/>
     <col min="10" max="10" width="33.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -757,7 +728,7 @@
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
-      <c r="F1" s="34"/>
+      <c r="F1" s="32"/>
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
     </row>
@@ -771,9 +742,9 @@
       <c r="E2" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="35"/>
+      <c r="F2" s="33"/>
       <c r="G2" s="13"/>
-      <c r="H2" s="31"/>
+      <c r="H2" s="29"/>
       <c r="I2" s="4"/>
       <c r="J2" s="1" t="s">
         <v>2</v>
@@ -797,14 +768,14 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="46.8" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="33"/>
-      <c r="B4" s="32"/>
+      <c r="A4" s="31"/>
+      <c r="B4" s="30"/>
       <c r="C4" s="18"/>
       <c r="D4" s="19"/>
       <c r="E4" s="9"/>
-      <c r="F4" s="29"/>
+      <c r="F4" s="27"/>
       <c r="G4" s="18"/>
-      <c r="H4" s="21"/>
+      <c r="H4" s="24"/>
       <c r="I4" s="7"/>
       <c r="J4" s="3" t="s">
         <v>4</v>
@@ -812,29 +783,29 @@
     </row>
     <row r="5" spans="1:10" ht="43.2" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5"/>
-      <c r="B5" s="22"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="19"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="11"/>
       <c r="F5" s="9" t="s">
         <v>12</v>
       </c>
       <c r="G5" s="15"/>
-      <c r="H5" s="25"/>
+      <c r="H5" s="23"/>
       <c r="J5" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="47.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5"/>
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="26"/>
+      <c r="C6" s="24"/>
       <c r="D6" s="16"/>
-      <c r="E6" s="30"/>
+      <c r="E6" s="28"/>
       <c r="F6" s="16"/>
-      <c r="G6" s="27"/>
+      <c r="G6" s="25"/>
       <c r="H6" s="9" t="s">
         <v>0</v>
       </c>
@@ -867,7 +838,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="J11" s="28" t="s">
+      <c r="J11" s="26" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
creation class perso + fin ini board
</commit_message>
<xml_diff>
--- a/map.xlsx
+++ b/map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loic-\OneDrive\Documents\GitHub\Projet-LO43\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{431F26AD-9D92-4329-AA84-9983D88D7D24}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{586435DC-6378-401E-9429-8A3EA98F0C6B}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="8_{431F26AD-9D92-4329-AA84-9983D88D7D24}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{7DB9426F-D211-4FAD-8B1E-8CE6D4DA8457}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" xr2:uid="{CBC8F156-E23D-49EC-AAE8-3A0909B6DE8A}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>S</t>
   </si>
@@ -714,7 +714,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -760,9 +760,7 @@
       <c r="E3" s="17"/>
       <c r="F3" s="18"/>
       <c r="G3" s="19"/>
-      <c r="H3" s="20" t="s">
-        <v>11</v>
-      </c>
+      <c r="H3" s="20"/>
       <c r="J3" s="2" t="s">
         <v>3</v>
       </c>

</xml_diff>